<commit_message>
create soundfont def fully working, need to add docstrings
</commit_message>
<xml_diff>
--- a/data/soundfont/viena_definition.xlsx
+++ b/data/soundfont/viena_definition.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W135"/>
+  <dimension ref="A1:X142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,17 +470,17 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>GONGS GIR OPEN</t>
+          <t>CALUNG DING1 OPEN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Gong OPEN.wav</t>
+          <t>Calung Ombak DING1.wav</t>
         </is>
       </c>
     </row>
@@ -488,17 +488,17 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GONGS PUR OPEN</t>
+          <t>CALUNG DONG1 OPEN</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Kempur OPEN.wav</t>
+          <t>Calung Ombak DONG1.wav</t>
         </is>
       </c>
     </row>
@@ -506,17 +506,17 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>GONGS TONG OPEN</t>
+          <t>CALUNG DENG1 OPEN</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Kemong OPEN.wav</t>
+          <t>Calung Ombak DENG1.wav</t>
         </is>
       </c>
     </row>
@@ -524,17 +524,17 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KEMPLI TICK OPEN</t>
+          <t>CALUNG DUNG1 OPEN</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Kempli MUTED.wav</t>
+          <t>Calung Ombak DUNG1.wav</t>
         </is>
       </c>
     </row>
@@ -542,17 +542,17 @@
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CENGCENG OPEN OPEN</t>
+          <t>CALUNG DANG1 OPEN</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Cengceng OPEN.wav</t>
+          <t>Calung Ombak DANG1.wav</t>
         </is>
       </c>
     </row>
@@ -560,17 +560,17 @@
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CENGCENG MUTED OPEN</t>
+          <t>CENGCENG OPEN OPEN</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Cengceng MUTED.wav</t>
+          <t>Cengceng OPEN.wav</t>
         </is>
       </c>
     </row>
@@ -578,17 +578,17 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KENDANG KA OPEN</t>
+          <t>CENGCENG MUTED OPEN</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Kendang KA wadon.wav</t>
+          <t>Cengceng MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -596,17 +596,17 @@
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>KENDANG PAK OPEN</t>
+          <t>GONGS GIR OPEN</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Kendang PAK lanang.wav</t>
+          <t>Gong OPEN.wav</t>
         </is>
       </c>
     </row>
@@ -614,17 +614,17 @@
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>KENDANG DE OPEN</t>
+          <t>GONGS PUR OPEN</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Kendang DE wadon.wav</t>
+          <t>Kempur OPEN.wav</t>
         </is>
       </c>
     </row>
@@ -632,17 +632,17 @@
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>KENDANG TUT OPEN</t>
+          <t>GONGS TONG OPEN</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Kendang TUT lanang.wav</t>
+          <t>Kemong OPEN.wav</t>
         </is>
       </c>
     </row>
@@ -650,17 +650,17 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KENDANG JU OPEN</t>
+          <t>JEGOGAN DING1 OPEN</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Kendang JU wadon.wav</t>
+          <t>Jegogan Ombak DING1.wav</t>
         </is>
       </c>
     </row>
@@ -668,17 +668,17 @@
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KENDANG KUNG OPEN</t>
+          <t>JEGOGAN DONG1 OPEN</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Kendang KUNG lanang.wav</t>
+          <t>Jegogan Ombak DONG1.wav</t>
         </is>
       </c>
     </row>
@@ -686,17 +686,17 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>JEGOGAN DING1 OPEN</t>
+          <t>JEGOGAN DENG1 OPEN</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Jegogan Ombak DING1.wav</t>
+          <t>Jegogan Ombak DENG1.wav</t>
         </is>
       </c>
     </row>
@@ -704,17 +704,17 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>JEGOGAN DONG1 OPEN</t>
+          <t>JEGOGAN DUNG1 OPEN</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Jegogan Ombak DONG1.wav</t>
+          <t>Jegogan Ombak DUNG1.wav</t>
         </is>
       </c>
     </row>
@@ -722,17 +722,17 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>JEGOGAN DENG1 OPEN</t>
+          <t>JEGOGAN DANG1 OPEN</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Jegogan Ombak DENG1.wav</t>
+          <t>Jegogan Ombak DANG1.wav</t>
         </is>
       </c>
     </row>
@@ -740,17 +740,17 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>JEGOGAN DUNG1 OPEN</t>
+          <t>KANTILAN DONG OPEN</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Jegogan Ombak DUNG1.wav</t>
+          <t>Kantilan Ombak DONG0.wav</t>
         </is>
       </c>
     </row>
@@ -758,17 +758,17 @@
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>JEGOGAN DANG1 OPEN</t>
+          <t>KANTILAN DONG MUTED</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Jegogan Ombak DANG1.wav</t>
+          <t>Kantilan Ombak DONG0_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -776,17 +776,17 @@
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CALUNG DING1 OPEN</t>
+          <t>KANTILAN DENG OPEN</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Calung Ombak DING1.wav</t>
+          <t>Kantilan Ombak DENG0.wav</t>
         </is>
       </c>
     </row>
@@ -794,17 +794,17 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CALUNG DONG1 OPEN</t>
+          <t>KANTILAN DENG MUTED</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Calung Ombak DONG1.wav</t>
+          <t>Kantilan Ombak DENG0_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -812,17 +812,17 @@
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CALUNG DENG1 OPEN</t>
+          <t>KANTILAN DUNG OPEN</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Calung Ombak DENG1.wav</t>
+          <t>Kantilan Ombak DUNG0.wav</t>
         </is>
       </c>
     </row>
@@ -830,17 +830,17 @@
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CALUNG DUNG1 OPEN</t>
+          <t>KANTILAN DUNG MUTED</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Calung Ombak DUNG1.wav</t>
+          <t>Kantilan Ombak DUNG0_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -848,17 +848,17 @@
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr">
         <is>
-          <t>CALUNG DANG1 OPEN</t>
+          <t>KANTILAN DANG OPEN</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Calung Ombak DANG1.wav</t>
+          <t>Kantilan Ombak DANG0.wav</t>
         </is>
       </c>
     </row>
@@ -866,17 +866,17 @@
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>REYONG DENG OPEN</t>
+          <t>KANTILAN DANG MUTED</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Reyong DENG0.wav</t>
+          <t>Kantilan Ombak DANG0_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -884,17 +884,17 @@
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr">
         <is>
-          <t>REYONG DUNG OPEN</t>
+          <t>KANTILAN DING1 OPEN</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Reyong DUNG0.wav</t>
+          <t>Kantilan Ombak DING1.wav</t>
         </is>
       </c>
     </row>
@@ -902,17 +902,17 @@
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr">
         <is>
-          <t>REYONG DANG OPEN</t>
+          <t>KANTILAN DING1 MUTED</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Reyong DANG0.wav</t>
+          <t>Kantilan Ombak DING1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -920,17 +920,17 @@
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>REYONG DING1 OPEN</t>
+          <t>KANTILAN DONG1 OPEN</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Reyong DING1.wav</t>
+          <t>Kantilan Ombak DONG1.wav</t>
         </is>
       </c>
     </row>
@@ -938,17 +938,17 @@
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>REYONG DENGDING OPEN</t>
+          <t>KANTILAN DONG1 MUTED</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Reyong DENG0-DING1.wav</t>
+          <t>Kantilan Ombak DONG1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -956,17 +956,17 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>REYONG DONG1 OPEN</t>
+          <t>KANTILAN DENG1 OPEN</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Reyong DONG1.wav</t>
+          <t>Kantilan Ombak DENG1.wav</t>
         </is>
       </c>
     </row>
@@ -974,17 +974,17 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>REYONG DENG1 OPEN</t>
+          <t>KANTILAN DENG1 MUTED</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Reyong DENG1.wav</t>
+          <t>Kantilan Ombak DENG1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -992,17 +992,17 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>REYONG DUNG1 OPEN</t>
+          <t>KANTILAN DUNG1 OPEN</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Reyong DUNG1.wav</t>
+          <t>Kantilan Ombak DUNG1.wav</t>
         </is>
       </c>
     </row>
@@ -1010,17 +1010,17 @@
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>REYONG DANG1 OPEN</t>
+          <t>KANTILAN DUNG1 MUTED</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Reyong DANG1.wav</t>
+          <t>Kantilan Ombak DUNG1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1028,17 +1028,17 @@
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
-          <t>REYONG DING2 OPEN</t>
+          <t>KANTILAN DANG1 OPEN</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="n">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Reyong DING2.wav</t>
+          <t>Kantilan Ombak DANG1.wav</t>
         </is>
       </c>
     </row>
@@ -1046,17 +1046,17 @@
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr">
         <is>
-          <t>REYONG DONG2 OPEN</t>
+          <t>KANTILAN DANG1 MUTED</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Reyong DONG2.wav</t>
+          <t>Kantilan Ombak DANG1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1064,17 +1064,17 @@
       <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr">
         <is>
-          <t>REYONG DENG2 OPEN</t>
+          <t>KANTILAN DING2 OPEN</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Reyong DENG2.wav</t>
+          <t>Kantilan Ombak DING2.wav</t>
         </is>
       </c>
     </row>
@@ -1082,17 +1082,17 @@
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>REYONG DUNG2 OPEN</t>
+          <t>KANTILAN DING2 MUTED</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Reyong DUNG2.wav</t>
+          <t>Kantilan Ombak DING2_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1100,17 +1100,17 @@
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr">
         <is>
-          <t>REYONG BYONG MUTED</t>
+          <t>KEMPLI TICK OPEN</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Reyong JET.wav</t>
+          <t>Kempli MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1118,17 +1118,17 @@
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr">
         <is>
-          <t>REYONG BYONG OPEN</t>
+          <t>KENDANG KA OPEN</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="n">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Reyong BYONG.wav</t>
+          <t>Kendang KA wadon.wav</t>
         </is>
       </c>
     </row>
@@ -1136,17 +1136,17 @@
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
-          <t>REYONG BYONG ABBREVIATED</t>
+          <t>KENDANG PAK OPEN</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Reyong BYOT.wav</t>
+          <t>Kendang PAK lanang.wav</t>
         </is>
       </c>
     </row>
@@ -1154,17 +1154,17 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>REYONG TICK OPEN</t>
+          <t>KENDANG DE OPEN</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="n">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Reyong TICK_1_PANGGUL.wav</t>
+          <t>Kendang DE wadon.wav</t>
         </is>
       </c>
     </row>
@@ -1172,17 +1172,17 @@
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>REYONG TICK_2_PANGGUL OPEN</t>
+          <t>KENDANG TUT OPEN</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="n">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Reyong TICK_2_PANGGUL.wav</t>
+          <t>Kendang TUT lanang.wav</t>
         </is>
       </c>
     </row>
@@ -1190,17 +1190,17 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>KANTILAN DONG OPEN</t>
+          <t>KENDANG JU OPEN</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="n">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DONG0.wav</t>
+          <t>Kendang JU wadon.wav</t>
         </is>
       </c>
     </row>
@@ -1208,17 +1208,17 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>KANTILAN DONG MUTED</t>
+          <t>KENDANG KUNG OPEN</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="n">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DONG0_MUTED.wav</t>
+          <t>Kendang KUNG lanang.wav</t>
         </is>
       </c>
     </row>
@@ -1226,17 +1226,17 @@
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
-          <t>KANTILAN DENG OPEN</t>
+          <t>PEMADE DONG OPEN</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DENG0.wav</t>
+          <t>Pemade Ombak DONG0.wav</t>
         </is>
       </c>
     </row>
@@ -1244,17 +1244,17 @@
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
-          <t>KANTILAN DENG MUTED</t>
+          <t>PEMADE DONG MUTED</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="n">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DENG0_MUTED.wav</t>
+          <t>Pemade Ombak DONG0_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1262,17 +1262,17 @@
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
-          <t>KANTILAN DUNG OPEN</t>
+          <t>PEMADE DENG OPEN</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="n">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DUNG0.wav</t>
+          <t>Pemade Ombak DENG0.wav</t>
         </is>
       </c>
     </row>
@@ -1280,17 +1280,17 @@
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
-          <t>KANTILAN DUNG MUTED</t>
+          <t>PEMADE DENG MUTED</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DUNG0_MUTED.wav</t>
+          <t>Pemade Ombak DENG0_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1298,17 +1298,17 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
-          <t>KANTILAN DANG OPEN</t>
+          <t>PEMADE DUNG OPEN</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="n">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DANG0.wav</t>
+          <t>Pemade Ombak DUNG0.wav</t>
         </is>
       </c>
     </row>
@@ -1316,17 +1316,17 @@
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr">
         <is>
-          <t>KANTILAN DANG MUTED</t>
+          <t>PEMADE DUNG MUTED</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="n">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DANG0_MUTED.wav</t>
+          <t>Pemade Ombak DUNG0_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1334,17 +1334,17 @@
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>KANTILAN DING1 OPEN</t>
+          <t>PEMADE DANG OPEN</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="n">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DING1.wav</t>
+          <t>Pemade Ombak DANG0.wav</t>
         </is>
       </c>
     </row>
@@ -1352,17 +1352,17 @@
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
-          <t>KANTILAN DING1 MUTED</t>
+          <t>PEMADE DANG MUTED</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DING1_MUTED.wav</t>
+          <t>Pemade Ombak DANG0_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1370,17 +1370,17 @@
       <c r="A52" t="inlineStr"/>
       <c r="B52" t="inlineStr">
         <is>
-          <t>KANTILAN DONG1 OPEN</t>
+          <t>PEMADE DING1 OPEN</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="n">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DONG1.wav</t>
+          <t>Pemade Ombak DING1.wav</t>
         </is>
       </c>
     </row>
@@ -1388,17 +1388,17 @@
       <c r="A53" t="inlineStr"/>
       <c r="B53" t="inlineStr">
         <is>
-          <t>KANTILAN DONG1 MUTED</t>
+          <t>PEMADE DING1 MUTED</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="n">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DONG1_MUTED.wav</t>
+          <t>Pemade Ombak DING1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1406,17 +1406,17 @@
       <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr">
         <is>
-          <t>KANTILAN DENG1 OPEN</t>
+          <t>PEMADE DONG1 OPEN</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="n">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DENG1.wav</t>
+          <t>Pemade Ombak DONG1.wav</t>
         </is>
       </c>
     </row>
@@ -1424,17 +1424,17 @@
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr">
         <is>
-          <t>KANTILAN DENG1 MUTED</t>
+          <t>PEMADE DONG1 MUTED</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="n">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DENG1_MUTED.wav</t>
+          <t>Pemade Ombak DONG1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1442,17 +1442,17 @@
       <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr">
         <is>
-          <t>KANTILAN DUNG1 OPEN</t>
+          <t>PEMADE DENG1 OPEN</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="n">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DUNG1.wav</t>
+          <t>Pemade Ombak DENG1.wav</t>
         </is>
       </c>
     </row>
@@ -1460,17 +1460,17 @@
       <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
-          <t>KANTILAN DUNG1 MUTED</t>
+          <t>PEMADE DENG1 MUTED</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="n">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DUNG1_MUTED.wav</t>
+          <t>Pemade Ombak DENG1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1478,17 +1478,17 @@
       <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr">
         <is>
-          <t>KANTILAN DANG1 OPEN</t>
+          <t>PEMADE DUNG1 OPEN</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="n">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DANG1.wav</t>
+          <t>Pemade Ombak DUNG1.wav</t>
         </is>
       </c>
     </row>
@@ -1496,17 +1496,17 @@
       <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr">
         <is>
-          <t>KANTILAN DANG1 MUTED</t>
+          <t>PEMADE DUNG1 MUTED</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="n">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DANG1_MUTED.wav</t>
+          <t>Pemade Ombak DUNG1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1514,17 +1514,17 @@
       <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr">
         <is>
-          <t>KANTILAN DING2 OPEN</t>
+          <t>PEMADE DANG1 OPEN</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="n">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DING2.wav</t>
+          <t>Pemade Ombak DANG1.wav</t>
         </is>
       </c>
     </row>
@@ -1532,17 +1532,17 @@
       <c r="A61" t="inlineStr"/>
       <c r="B61" t="inlineStr">
         <is>
-          <t>KANTILAN DING2 MUTED</t>
+          <t>PEMADE DANG1 MUTED</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="n">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Kantilan Ombak DING2_MUTED.wav</t>
+          <t>Pemade Ombak DANG1_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1550,17 +1550,17 @@
       <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr">
         <is>
-          <t>PEMADE DONG OPEN</t>
+          <t>PEMADE DING2 OPEN</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="n">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Pemade Ombak DONG0.wav</t>
+          <t>Pemade Ombak DING2.wav</t>
         </is>
       </c>
     </row>
@@ -1568,17 +1568,17 @@
       <c r="A63" t="inlineStr"/>
       <c r="B63" t="inlineStr">
         <is>
-          <t>PEMADE DONG MUTED</t>
+          <t>PEMADE DING2 MUTED</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="n">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Pemade Ombak DONG0_MUTED.wav</t>
+          <t>Pemade Ombak DING2_MUTED.wav</t>
         </is>
       </c>
     </row>
@@ -1586,17 +1586,17 @@
       <c r="A64" t="inlineStr"/>
       <c r="B64" t="inlineStr">
         <is>
-          <t>PEMADE DENG OPEN</t>
+          <t>REYONG DENG OPEN</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="n">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Pemade Ombak DENG0.wav</t>
+          <t>Reyong DENG0.wav</t>
         </is>
       </c>
     </row>
@@ -1604,17 +1604,17 @@
       <c r="A65" t="inlineStr"/>
       <c r="B65" t="inlineStr">
         <is>
-          <t>PEMADE DENG MUTED</t>
+          <t>REYONG DUNG OPEN</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="n">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Pemade Ombak DENG0_MUTED.wav</t>
+          <t>Reyong DUNG0.wav</t>
         </is>
       </c>
     </row>
@@ -1622,17 +1622,17 @@
       <c r="A66" t="inlineStr"/>
       <c r="B66" t="inlineStr">
         <is>
-          <t>PEMADE DUNG OPEN</t>
+          <t>REYONG DANG OPEN</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="n">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Pemade Ombak DUNG0.wav</t>
+          <t>Reyong DANG0.wav</t>
         </is>
       </c>
     </row>
@@ -1640,17 +1640,17 @@
       <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr">
         <is>
-          <t>PEMADE DUNG MUTED</t>
+          <t>REYONG DING1 OPEN</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="n">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Pemade Ombak DUNG0_MUTED.wav</t>
+          <t>Reyong DING1.wav</t>
         </is>
       </c>
     </row>
@@ -1658,17 +1658,17 @@
       <c r="A68" t="inlineStr"/>
       <c r="B68" t="inlineStr">
         <is>
-          <t>PEMADE DANG OPEN</t>
+          <t>REYONG DENGDING OPEN</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="n">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Pemade Ombak DANG0.wav</t>
+          <t>Reyong DENG0-DING1.wav</t>
         </is>
       </c>
     </row>
@@ -1676,17 +1676,17 @@
       <c r="A69" t="inlineStr"/>
       <c r="B69" t="inlineStr">
         <is>
-          <t>PEMADE DANG MUTED</t>
+          <t>REYONG DONG1 OPEN</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="n">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Pemade Ombak DANG0_MUTED.wav</t>
+          <t>Reyong DONG1.wav</t>
         </is>
       </c>
     </row>
@@ -1694,17 +1694,17 @@
       <c r="A70" t="inlineStr"/>
       <c r="B70" t="inlineStr">
         <is>
-          <t>PEMADE DING1 OPEN</t>
+          <t>REYONG DENG1 OPEN</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="n">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Pemade Ombak DING1.wav</t>
+          <t>Reyong DENG1.wav</t>
         </is>
       </c>
     </row>
@@ -1712,17 +1712,17 @@
       <c r="A71" t="inlineStr"/>
       <c r="B71" t="inlineStr">
         <is>
-          <t>PEMADE DING1 MUTED</t>
+          <t>REYONG DUNG1 OPEN</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="n">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Pemade Ombak DING1_MUTED.wav</t>
+          <t>Reyong DUNG1.wav</t>
         </is>
       </c>
     </row>
@@ -1730,17 +1730,17 @@
       <c r="A72" t="inlineStr"/>
       <c r="B72" t="inlineStr">
         <is>
-          <t>PEMADE DONG1 OPEN</t>
+          <t>REYONG DANG1 OPEN</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="n">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Pemade Ombak DONG1.wav</t>
+          <t>Reyong DANG1.wav</t>
         </is>
       </c>
     </row>
@@ -1748,17 +1748,17 @@
       <c r="A73" t="inlineStr"/>
       <c r="B73" t="inlineStr">
         <is>
-          <t>PEMADE DONG1 MUTED</t>
+          <t>REYONG DING2 OPEN</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="n">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Pemade Ombak DONG1_MUTED.wav</t>
+          <t>Reyong DING2.wav</t>
         </is>
       </c>
     </row>
@@ -1766,17 +1766,17 @@
       <c r="A74" t="inlineStr"/>
       <c r="B74" t="inlineStr">
         <is>
-          <t>PEMADE DENG1 OPEN</t>
+          <t>REYONG DONG2 OPEN</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="n">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Pemade Ombak DENG1.wav</t>
+          <t>Reyong DONG2.wav</t>
         </is>
       </c>
     </row>
@@ -1784,17 +1784,17 @@
       <c r="A75" t="inlineStr"/>
       <c r="B75" t="inlineStr">
         <is>
-          <t>PEMADE DENG1 MUTED</t>
+          <t>REYONG DENG2 OPEN</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="n">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Pemade Ombak DENG1_MUTED.wav</t>
+          <t>Reyong DENG2.wav</t>
         </is>
       </c>
     </row>
@@ -1802,17 +1802,17 @@
       <c r="A76" t="inlineStr"/>
       <c r="B76" t="inlineStr">
         <is>
-          <t>PEMADE DUNG1 OPEN</t>
+          <t>REYONG DUNG2 OPEN</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="n">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Pemade Ombak DUNG1.wav</t>
+          <t>Reyong DUNG2.wav</t>
         </is>
       </c>
     </row>
@@ -1820,17 +1820,17 @@
       <c r="A77" t="inlineStr"/>
       <c r="B77" t="inlineStr">
         <is>
-          <t>PEMADE DUNG1 MUTED</t>
+          <t>REYONG BYONG MUTED</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="n">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Pemade Ombak DUNG1_MUTED.wav</t>
+          <t>Reyong JET.wav</t>
         </is>
       </c>
     </row>
@@ -1838,17 +1838,17 @@
       <c r="A78" t="inlineStr"/>
       <c r="B78" t="inlineStr">
         <is>
-          <t>PEMADE DANG1 OPEN</t>
+          <t>REYONG BYONG OPEN</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="n">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Pemade Ombak DANG1.wav</t>
+          <t>Reyong BYONG.wav</t>
         </is>
       </c>
     </row>
@@ -1856,17 +1856,17 @@
       <c r="A79" t="inlineStr"/>
       <c r="B79" t="inlineStr">
         <is>
-          <t>PEMADE DANG1 MUTED</t>
+          <t>REYONG BYONG ABBREVIATED</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="n">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Pemade Ombak DANG1_MUTED.wav</t>
+          <t>Reyong BYOT.wav</t>
         </is>
       </c>
     </row>
@@ -1874,17 +1874,17 @@
       <c r="A80" t="inlineStr"/>
       <c r="B80" t="inlineStr">
         <is>
-          <t>PEMADE DING2 OPEN</t>
+          <t>REYONG TICK OPEN</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="n">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Pemade Ombak DING2.wav</t>
+          <t>Reyong TICK_1_PANGGUL.wav</t>
         </is>
       </c>
     </row>
@@ -1892,17 +1892,17 @@
       <c r="A81" t="inlineStr"/>
       <c r="B81" t="inlineStr">
         <is>
-          <t>PEMADE DING2 MUTED</t>
+          <t>REYONG TICK_2_PANGGUL OPEN</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="n">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Pemade Ombak DING2_MUTED.wav</t>
+          <t>Reyong TICK_2_PANGGUL.wav</t>
         </is>
       </c>
     </row>
@@ -2128,7 +2128,7 @@
       <c r="A95" t="inlineStr"/>
       <c r="B95" t="inlineStr">
         <is>
-          <t>GONGS</t>
+          <t>CALUNG</t>
         </is>
       </c>
     </row>
@@ -2142,17 +2142,32 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>GONGS GIR OPEN</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>GONGS PUR OPEN</t>
+          <t>CALUNG DING1 OPEN</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>GONGS TONG OPEN</t>
+          <t>CALUNG DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>CALUNG DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>CALUNG DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>CALUNG DANG1 OPEN</t>
         </is>
       </c>
     </row>
@@ -2166,17 +2181,27 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>25-25</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>26-26</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>3-3</t>
+          <t>27-27</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>28-28</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>29-29</t>
         </is>
       </c>
     </row>
@@ -2189,20 +2214,26 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F98" t="n">
-        <v>3</v>
+        <v>27</v>
+      </c>
+      <c r="G98" t="n">
+        <v>28</v>
+      </c>
+      <c r="H98" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr"/>
       <c r="B99" t="inlineStr">
         <is>
-          <t>JEGOGAN</t>
+          <t>CENGCENG</t>
         </is>
       </c>
     </row>
@@ -2216,27 +2247,17 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>JEGOGAN DING1 OPEN</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>JEGOGAN DONG1 OPEN</t>
+          <t>CENGCENG OPEN OPEN</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>JEGOGAN DENG1 OPEN</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>JEGOGAN DUNG1 OPEN</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>JEGOGAN DANG1 OPEN</t>
+          <t>CENGCENG MUTED OPEN</t>
         </is>
       </c>
     </row>
@@ -2250,27 +2271,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>20-20</t>
+          <t>5-5</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>21-21</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>22-22</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>23-23</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>24-24</t>
+          <t>6-6</t>
         </is>
       </c>
     </row>
@@ -2283,26 +2289,17 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E102" t="n">
-        <v>21</v>
-      </c>
-      <c r="F102" t="n">
-        <v>22</v>
-      </c>
-      <c r="G102" t="n">
-        <v>23</v>
-      </c>
-      <c r="H102" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr"/>
       <c r="B103" t="inlineStr">
         <is>
-          <t>PEMADE</t>
+          <t>GONGS</t>
         </is>
       </c>
     </row>
@@ -2316,102 +2313,22 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>PEMADE DONG OPEN</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>PEMADE DONG MUTED</t>
+          <t>GONGS GIR OPEN</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>PEMADE DENG OPEN</t>
+          <t>GONGS PUR OPEN</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>PEMADE DENG MUTED</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>PEMADE DUNG OPEN</t>
-        </is>
-      </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>PEMADE DUNG MUTED</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>PEMADE DANG OPEN</t>
-        </is>
-      </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>PEMADE DANG MUTED</t>
-        </is>
-      </c>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>PEMADE DING1 OPEN</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>PEMADE DING1 MUTED</t>
-        </is>
-      </c>
-      <c r="N104" t="inlineStr">
-        <is>
-          <t>PEMADE DONG1 OPEN</t>
-        </is>
-      </c>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>PEMADE DONG1 MUTED</t>
-        </is>
-      </c>
-      <c r="P104" t="inlineStr">
-        <is>
-          <t>PEMADE DENG1 OPEN</t>
-        </is>
-      </c>
-      <c r="Q104" t="inlineStr">
-        <is>
-          <t>PEMADE DENG1 MUTED</t>
-        </is>
-      </c>
-      <c r="R104" t="inlineStr">
-        <is>
-          <t>PEMADE DUNG1 OPEN</t>
-        </is>
-      </c>
-      <c r="S104" t="inlineStr">
-        <is>
-          <t>PEMADE DUNG1 MUTED</t>
-        </is>
-      </c>
-      <c r="T104" t="inlineStr">
-        <is>
-          <t>PEMADE DANG1 OPEN</t>
-        </is>
-      </c>
-      <c r="U104" t="inlineStr">
-        <is>
-          <t>PEMADE DANG1 MUTED</t>
-        </is>
-      </c>
-      <c r="V104" t="inlineStr">
-        <is>
-          <t>PEMADE DING2 OPEN</t>
-        </is>
-      </c>
-      <c r="W104" t="inlineStr">
-        <is>
-          <t>PEMADE DING2 MUTED</t>
+          <t>GONGS TONG OPEN</t>
         </is>
       </c>
     </row>
@@ -2425,102 +2342,17 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>75-75</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>76-76</t>
+          <t>2-2</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>77-77</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>78-78</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>79-79</t>
-        </is>
-      </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>80-80</t>
-        </is>
-      </c>
-      <c r="J105" t="inlineStr">
-        <is>
-          <t>81-81</t>
-        </is>
-      </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>82-82</t>
-        </is>
-      </c>
-      <c r="L105" t="inlineStr">
-        <is>
-          <t>83-83</t>
-        </is>
-      </c>
-      <c r="M105" t="inlineStr">
-        <is>
-          <t>84-84</t>
-        </is>
-      </c>
-      <c r="N105" t="inlineStr">
-        <is>
-          <t>85-85</t>
-        </is>
-      </c>
-      <c r="O105" t="inlineStr">
-        <is>
-          <t>86-86</t>
-        </is>
-      </c>
-      <c r="P105" t="inlineStr">
-        <is>
-          <t>87-87</t>
-        </is>
-      </c>
-      <c r="Q105" t="inlineStr">
-        <is>
-          <t>88-88</t>
-        </is>
-      </c>
-      <c r="R105" t="inlineStr">
-        <is>
-          <t>89-89</t>
-        </is>
-      </c>
-      <c r="S105" t="inlineStr">
-        <is>
-          <t>90-90</t>
-        </is>
-      </c>
-      <c r="T105" t="inlineStr">
-        <is>
-          <t>91-91</t>
-        </is>
-      </c>
-      <c r="U105" t="inlineStr">
-        <is>
-          <t>92-92</t>
-        </is>
-      </c>
-      <c r="V105" t="inlineStr">
-        <is>
-          <t>93-93</t>
-        </is>
-      </c>
-      <c r="W105" t="inlineStr">
-        <is>
-          <t>94-94</t>
+          <t>3-3</t>
         </is>
       </c>
     </row>
@@ -2533,71 +2365,20 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="E106" t="n">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="F106" t="n">
-        <v>77</v>
-      </c>
-      <c r="G106" t="n">
-        <v>78</v>
-      </c>
-      <c r="H106" t="n">
-        <v>79</v>
-      </c>
-      <c r="I106" t="n">
-        <v>80</v>
-      </c>
-      <c r="J106" t="n">
-        <v>81</v>
-      </c>
-      <c r="K106" t="n">
-        <v>82</v>
-      </c>
-      <c r="L106" t="n">
-        <v>83</v>
-      </c>
-      <c r="M106" t="n">
-        <v>84</v>
-      </c>
-      <c r="N106" t="n">
-        <v>85</v>
-      </c>
-      <c r="O106" t="n">
-        <v>86</v>
-      </c>
-      <c r="P106" t="n">
-        <v>87</v>
-      </c>
-      <c r="Q106" t="n">
-        <v>88</v>
-      </c>
-      <c r="R106" t="n">
-        <v>89</v>
-      </c>
-      <c r="S106" t="n">
-        <v>90</v>
-      </c>
-      <c r="T106" t="n">
-        <v>91</v>
-      </c>
-      <c r="U106" t="n">
-        <v>92</v>
-      </c>
-      <c r="V106" t="n">
-        <v>93</v>
-      </c>
-      <c r="W106" t="n">
-        <v>94</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr"/>
       <c r="B107" t="inlineStr">
         <is>
-          <t>KEMPLI</t>
+          <t>JEGOGAN</t>
         </is>
       </c>
     </row>
@@ -2611,7 +2392,32 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>KEMPLI TICK OPEN</t>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>JEGOGAN DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>JEGOGAN DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>JEGOGAN DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>JEGOGAN DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>JEGOGAN DANG1 OPEN</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2431,27 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>4-4</t>
+          <t>20-20</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>21-21</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>22-22</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>23-23</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>24-24</t>
         </is>
       </c>
     </row>
@@ -2638,14 +2464,26 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="E110" t="n">
+        <v>21</v>
+      </c>
+      <c r="F110" t="n">
+        <v>22</v>
+      </c>
+      <c r="G110" t="n">
+        <v>23</v>
+      </c>
+      <c r="H110" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr"/>
       <c r="B111" t="inlineStr">
         <is>
-          <t>CALUNG</t>
+          <t>KANTILAN</t>
         </is>
       </c>
     </row>
@@ -2659,27 +2497,107 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>CALUNG DING1 OPEN</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>CALUNG DONG1 OPEN</t>
+          <t>KANTILAN DONG OPEN</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>CALUNG DENG1 OPEN</t>
+          <t>KANTILAN DONG MUTED</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>CALUNG DUNG1 OPEN</t>
+          <t>KANTILAN DENG OPEN</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>CALUNG DANG1 OPEN</t>
+          <t>KANTILAN DENG MUTED</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>KANTILAN DUNG OPEN</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>KANTILAN DUNG MUTED</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>KANTILAN DANG OPEN</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>KANTILAN DANG MUTED</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>KANTILAN DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>KANTILAN DING1 MUTED</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>KANTILAN DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>KANTILAN DONG1 MUTED</t>
+        </is>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>KANTILAN DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="R112" t="inlineStr">
+        <is>
+          <t>KANTILAN DENG1 MUTED</t>
+        </is>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>KANTILAN DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="T112" t="inlineStr">
+        <is>
+          <t>KANTILAN DUNG1 MUTED</t>
+        </is>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>KANTILAN DANG1 OPEN</t>
+        </is>
+      </c>
+      <c r="V112" t="inlineStr">
+        <is>
+          <t>KANTILAN DANG1 MUTED</t>
+        </is>
+      </c>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>KANTILAN DING2 OPEN</t>
+        </is>
+      </c>
+      <c r="X112" t="inlineStr">
+        <is>
+          <t>KANTILAN DING2 MUTED</t>
         </is>
       </c>
     </row>
@@ -2693,27 +2611,102 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>25-25</t>
+          <t>55-55</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>26-26</t>
+          <t>56-56</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>27-27</t>
+          <t>57-57</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>28-28</t>
+          <t>58-58</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>29-29</t>
+          <t>59-59</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>60-60</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>61-61</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>62-62</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>63-63</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>64-64</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>65-65</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>66-66</t>
+        </is>
+      </c>
+      <c r="P113" t="inlineStr">
+        <is>
+          <t>67-67</t>
+        </is>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>68-68</t>
+        </is>
+      </c>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>69-69</t>
+        </is>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>70-70</t>
+        </is>
+      </c>
+      <c r="T113" t="inlineStr">
+        <is>
+          <t>71-71</t>
+        </is>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>72-72</t>
+        </is>
+      </c>
+      <c r="V113" t="inlineStr">
+        <is>
+          <t>73-73</t>
+        </is>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>74-74</t>
         </is>
       </c>
     </row>
@@ -2726,26 +2719,71 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E114" t="n">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="F114" t="n">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="G114" t="n">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="H114" t="n">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="I114" t="n">
+        <v>60</v>
+      </c>
+      <c r="J114" t="n">
+        <v>61</v>
+      </c>
+      <c r="K114" t="n">
+        <v>62</v>
+      </c>
+      <c r="L114" t="n">
+        <v>63</v>
+      </c>
+      <c r="M114" t="n">
+        <v>64</v>
+      </c>
+      <c r="N114" t="n">
+        <v>65</v>
+      </c>
+      <c r="O114" t="n">
+        <v>66</v>
+      </c>
+      <c r="P114" t="n">
+        <v>67</v>
+      </c>
+      <c r="Q114" t="n">
+        <v>68</v>
+      </c>
+      <c r="R114" t="n">
+        <v>69</v>
+      </c>
+      <c r="S114" t="n">
+        <v>70</v>
+      </c>
+      <c r="T114" t="n">
+        <v>71</v>
+      </c>
+      <c r="U114" t="n">
+        <v>72</v>
+      </c>
+      <c r="V114" t="n">
+        <v>73</v>
+      </c>
+      <c r="W114" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr"/>
       <c r="B115" t="inlineStr">
         <is>
-          <t>KANTILAN</t>
+          <t>KEMPLI</t>
         </is>
       </c>
     </row>
@@ -2759,102 +2797,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>KANTILAN DONG OPEN</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>KANTILAN DONG MUTED</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>KANTILAN DENG OPEN</t>
-        </is>
-      </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>KANTILAN DENG MUTED</t>
-        </is>
-      </c>
-      <c r="H116" t="inlineStr">
-        <is>
-          <t>KANTILAN DUNG OPEN</t>
-        </is>
-      </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>KANTILAN DUNG MUTED</t>
-        </is>
-      </c>
-      <c r="J116" t="inlineStr">
-        <is>
-          <t>KANTILAN DANG OPEN</t>
-        </is>
-      </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>KANTILAN DANG MUTED</t>
-        </is>
-      </c>
-      <c r="L116" t="inlineStr">
-        <is>
-          <t>KANTILAN DING1 OPEN</t>
-        </is>
-      </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>KANTILAN DING1 MUTED</t>
-        </is>
-      </c>
-      <c r="N116" t="inlineStr">
-        <is>
-          <t>KANTILAN DONG1 OPEN</t>
-        </is>
-      </c>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>KANTILAN DONG1 MUTED</t>
-        </is>
-      </c>
-      <c r="P116" t="inlineStr">
-        <is>
-          <t>KANTILAN DENG1 OPEN</t>
-        </is>
-      </c>
-      <c r="Q116" t="inlineStr">
-        <is>
-          <t>KANTILAN DENG1 MUTED</t>
-        </is>
-      </c>
-      <c r="R116" t="inlineStr">
-        <is>
-          <t>KANTILAN DUNG1 OPEN</t>
-        </is>
-      </c>
-      <c r="S116" t="inlineStr">
-        <is>
-          <t>KANTILAN DUNG1 MUTED</t>
-        </is>
-      </c>
-      <c r="T116" t="inlineStr">
-        <is>
-          <t>KANTILAN DANG1 OPEN</t>
-        </is>
-      </c>
-      <c r="U116" t="inlineStr">
-        <is>
-          <t>KANTILAN DANG1 MUTED</t>
-        </is>
-      </c>
-      <c r="V116" t="inlineStr">
-        <is>
-          <t>KANTILAN DING2 OPEN</t>
-        </is>
-      </c>
-      <c r="W116" t="inlineStr">
-        <is>
-          <t>KANTILAN DING2 MUTED</t>
+          <t>KEMPLI TICK OPEN</t>
         </is>
       </c>
     </row>
@@ -2868,102 +2816,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>55-55</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>56-56</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>57-57</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>58-58</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t>59-59</t>
-        </is>
-      </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>60-60</t>
-        </is>
-      </c>
-      <c r="J117" t="inlineStr">
-        <is>
-          <t>61-61</t>
-        </is>
-      </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>62-62</t>
-        </is>
-      </c>
-      <c r="L117" t="inlineStr">
-        <is>
-          <t>63-63</t>
-        </is>
-      </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>64-64</t>
-        </is>
-      </c>
-      <c r="N117" t="inlineStr">
-        <is>
-          <t>65-65</t>
-        </is>
-      </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>66-66</t>
-        </is>
-      </c>
-      <c r="P117" t="inlineStr">
-        <is>
-          <t>67-67</t>
-        </is>
-      </c>
-      <c r="Q117" t="inlineStr">
-        <is>
-          <t>68-68</t>
-        </is>
-      </c>
-      <c r="R117" t="inlineStr">
-        <is>
-          <t>69-69</t>
-        </is>
-      </c>
-      <c r="S117" t="inlineStr">
-        <is>
-          <t>70-70</t>
-        </is>
-      </c>
-      <c r="T117" t="inlineStr">
-        <is>
-          <t>71-71</t>
-        </is>
-      </c>
-      <c r="U117" t="inlineStr">
-        <is>
-          <t>72-72</t>
-        </is>
-      </c>
-      <c r="V117" t="inlineStr">
-        <is>
-          <t>73-73</t>
-        </is>
-      </c>
-      <c r="W117" t="inlineStr">
-        <is>
-          <t>74-74</t>
+          <t>4-4</t>
         </is>
       </c>
     </row>
@@ -2976,64 +2829,7 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>55</v>
-      </c>
-      <c r="E118" t="n">
-        <v>56</v>
-      </c>
-      <c r="F118" t="n">
-        <v>57</v>
-      </c>
-      <c r="G118" t="n">
-        <v>58</v>
-      </c>
-      <c r="H118" t="n">
-        <v>59</v>
-      </c>
-      <c r="I118" t="n">
-        <v>60</v>
-      </c>
-      <c r="J118" t="n">
-        <v>61</v>
-      </c>
-      <c r="K118" t="n">
-        <v>62</v>
-      </c>
-      <c r="L118" t="n">
-        <v>63</v>
-      </c>
-      <c r="M118" t="n">
-        <v>64</v>
-      </c>
-      <c r="N118" t="n">
-        <v>65</v>
-      </c>
-      <c r="O118" t="n">
-        <v>66</v>
-      </c>
-      <c r="P118" t="n">
-        <v>67</v>
-      </c>
-      <c r="Q118" t="n">
-        <v>68</v>
-      </c>
-      <c r="R118" t="n">
-        <v>69</v>
-      </c>
-      <c r="S118" t="n">
-        <v>70</v>
-      </c>
-      <c r="T118" t="n">
-        <v>71</v>
-      </c>
-      <c r="U118" t="n">
-        <v>72</v>
-      </c>
-      <c r="V118" t="n">
-        <v>73</v>
-      </c>
-      <c r="W118" t="n">
-        <v>74</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119">
@@ -3054,30 +2850,35 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
           <t>KENDANG KA OPEN</t>
         </is>
       </c>
-      <c r="E120" t="inlineStr">
+      <c r="F120" t="inlineStr">
         <is>
           <t>KENDANG PAK OPEN</t>
         </is>
       </c>
-      <c r="F120" t="inlineStr">
+      <c r="G120" t="inlineStr">
         <is>
           <t>KENDANG DE OPEN</t>
         </is>
       </c>
-      <c r="G120" t="inlineStr">
+      <c r="H120" t="inlineStr">
         <is>
           <t>KENDANG TUT OPEN</t>
         </is>
       </c>
-      <c r="H120" t="inlineStr">
+      <c r="I120" t="inlineStr">
         <is>
           <t>KENDANG JU OPEN</t>
         </is>
       </c>
-      <c r="I120" t="inlineStr">
+      <c r="J120" t="inlineStr">
         <is>
           <t>KENDANG KUNG OPEN</t>
         </is>
@@ -3153,7 +2954,7 @@
       <c r="A123" t="inlineStr"/>
       <c r="B123" t="inlineStr">
         <is>
-          <t>REYONG</t>
+          <t>PEMADE</t>
         </is>
       </c>
     </row>
@@ -3167,92 +2968,107 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>REYONG DENG OPEN</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>REYONG DUNG OPEN</t>
+          <t>PEMADE DONG OPEN</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>REYONG DANG OPEN</t>
+          <t>PEMADE DONG MUTED</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>REYONG DING1 OPEN</t>
+          <t>PEMADE DENG OPEN</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>REYONG DENGDING OPEN</t>
+          <t>PEMADE DENG MUTED</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>REYONG DONG1 OPEN</t>
+          <t>PEMADE DUNG OPEN</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>REYONG DENG1 OPEN</t>
+          <t>PEMADE DUNG MUTED</t>
         </is>
       </c>
       <c r="K124" t="inlineStr">
         <is>
-          <t>REYONG DUNG1 OPEN</t>
+          <t>PEMADE DANG OPEN</t>
         </is>
       </c>
       <c r="L124" t="inlineStr">
         <is>
-          <t>REYONG DANG1 OPEN</t>
+          <t>PEMADE DANG MUTED</t>
         </is>
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>REYONG DING2 OPEN</t>
+          <t>PEMADE DING1 OPEN</t>
         </is>
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>REYONG DONG2 OPEN</t>
+          <t>PEMADE DING1 MUTED</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
         <is>
-          <t>REYONG DENG2 OPEN</t>
+          <t>PEMADE DONG1 OPEN</t>
         </is>
       </c>
       <c r="P124" t="inlineStr">
         <is>
-          <t>REYONG DUNG2 OPEN</t>
+          <t>PEMADE DONG1 MUTED</t>
         </is>
       </c>
       <c r="Q124" t="inlineStr">
         <is>
-          <t>REYONG BYONG MUTED</t>
+          <t>PEMADE DENG1 OPEN</t>
         </is>
       </c>
       <c r="R124" t="inlineStr">
         <is>
-          <t>REYONG BYONG OPEN</t>
+          <t>PEMADE DENG1 MUTED</t>
         </is>
       </c>
       <c r="S124" t="inlineStr">
         <is>
-          <t>REYONG BYONG ABBREVIATED</t>
+          <t>PEMADE DUNG1 OPEN</t>
         </is>
       </c>
       <c r="T124" t="inlineStr">
         <is>
-          <t>REYONG TICK OPEN</t>
+          <t>PEMADE DUNG1 MUTED</t>
         </is>
       </c>
       <c r="U124" t="inlineStr">
         <is>
-          <t>REYONG TICK_2_PANGGUL OPEN</t>
+          <t>PEMADE DANG1 OPEN</t>
+        </is>
+      </c>
+      <c r="V124" t="inlineStr">
+        <is>
+          <t>PEMADE DANG1 MUTED</t>
+        </is>
+      </c>
+      <c r="W124" t="inlineStr">
+        <is>
+          <t>PEMADE DING2 OPEN</t>
+        </is>
+      </c>
+      <c r="X124" t="inlineStr">
+        <is>
+          <t>PEMADE DING2 MUTED</t>
         </is>
       </c>
     </row>
@@ -3266,92 +3082,102 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>30-30</t>
+          <t>75-75</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>31-31</t>
+          <t>76-76</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>32-32</t>
+          <t>77-77</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>33-33</t>
+          <t>78-78</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>34-34</t>
+          <t>79-79</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>35-35</t>
+          <t>80-80</t>
         </is>
       </c>
       <c r="J125" t="inlineStr">
         <is>
-          <t>36-36</t>
+          <t>81-81</t>
         </is>
       </c>
       <c r="K125" t="inlineStr">
         <is>
-          <t>37-37</t>
+          <t>82-82</t>
         </is>
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>38-38</t>
+          <t>83-83</t>
         </is>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>39-39</t>
+          <t>84-84</t>
         </is>
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>40-40</t>
+          <t>85-85</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
         <is>
-          <t>41-41</t>
+          <t>86-86</t>
         </is>
       </c>
       <c r="P125" t="inlineStr">
         <is>
-          <t>42-42</t>
+          <t>87-87</t>
         </is>
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>43-43</t>
+          <t>88-88</t>
         </is>
       </c>
       <c r="R125" t="inlineStr">
         <is>
-          <t>44-44</t>
+          <t>89-89</t>
         </is>
       </c>
       <c r="S125" t="inlineStr">
         <is>
-          <t>45-45</t>
+          <t>90-90</t>
         </is>
       </c>
       <c r="T125" t="inlineStr">
         <is>
-          <t>46-46</t>
+          <t>91-91</t>
         </is>
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>47-47</t>
+          <t>92-92</t>
+        </is>
+      </c>
+      <c r="V125" t="inlineStr">
+        <is>
+          <t>93-93</t>
+        </is>
+      </c>
+      <c r="W125" t="inlineStr">
+        <is>
+          <t>94-94</t>
         </is>
       </c>
     </row>
@@ -3364,65 +3190,71 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="E126" t="n">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="F126" t="n">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="G126" t="n">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="H126" t="n">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="I126" t="n">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="J126" t="n">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="K126" t="n">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="L126" t="n">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="M126" t="n">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="N126" t="n">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="O126" t="n">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="P126" t="n">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="Q126" t="n">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="R126" t="n">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="S126" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="T126" t="n">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="U126" t="n">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="V126" t="n">
+        <v>93</v>
+      </c>
+      <c r="W126" t="n">
+        <v>94</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr"/>
       <c r="B127" t="inlineStr">
         <is>
-          <t>UGAL</t>
+          <t>REYONG</t>
         </is>
       </c>
     </row>
@@ -3436,52 +3268,97 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>UGAL DONG OPEN</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>UGAL DENG OPEN</t>
+          <t>REYONG DENG OPEN</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>UGAL DUNG OPEN</t>
+          <t>REYONG DUNG OPEN</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>UGAL DANG OPEN</t>
+          <t>REYONG DANG OPEN</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>UGAL DING1 OPEN</t>
+          <t>REYONG DING1 OPEN</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>UGAL DONG1 OPEN</t>
+          <t>REYONG DENGDING OPEN</t>
         </is>
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>UGAL DENG1 OPEN</t>
+          <t>REYONG DONG1 OPEN</t>
         </is>
       </c>
       <c r="K128" t="inlineStr">
         <is>
-          <t>UGAL DUNG1 OPEN</t>
+          <t>REYONG DENG1 OPEN</t>
         </is>
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>UGAL DANG1 OPEN</t>
+          <t>REYONG DUNG1 OPEN</t>
         </is>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>UGAL DING2 OPEN</t>
+          <t>REYONG DANG1 OPEN</t>
+        </is>
+      </c>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>REYONG DING2 OPEN</t>
+        </is>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>REYONG DONG2 OPEN</t>
+        </is>
+      </c>
+      <c r="P128" t="inlineStr">
+        <is>
+          <t>REYONG DENG2 OPEN</t>
+        </is>
+      </c>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>REYONG DUNG2 OPEN</t>
+        </is>
+      </c>
+      <c r="R128" t="inlineStr">
+        <is>
+          <t>REYONG BYONG MUTED</t>
+        </is>
+      </c>
+      <c r="S128" t="inlineStr">
+        <is>
+          <t>REYONG BYONG OPEN</t>
+        </is>
+      </c>
+      <c r="T128" t="inlineStr">
+        <is>
+          <t>REYONG BYONG ABBREVIATED</t>
+        </is>
+      </c>
+      <c r="U128" t="inlineStr">
+        <is>
+          <t>REYONG TICK OPEN</t>
+        </is>
+      </c>
+      <c r="V128" t="inlineStr">
+        <is>
+          <t>REYONG TICK_2_PANGGUL OPEN</t>
         </is>
       </c>
     </row>
@@ -3495,52 +3372,92 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>95-95</t>
+          <t>30-30</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>96-96</t>
+          <t>31-31</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>97-97</t>
+          <t>32-32</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>98-98</t>
+          <t>33-33</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>99-99</t>
+          <t>34-34</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>100-100</t>
+          <t>35-35</t>
         </is>
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>101-101</t>
+          <t>36-36</t>
         </is>
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>102-102</t>
+          <t>37-37</t>
         </is>
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>103-103</t>
+          <t>38-38</t>
         </is>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>104-104</t>
+          <t>39-39</t>
+        </is>
+      </c>
+      <c r="N129" t="inlineStr">
+        <is>
+          <t>40-40</t>
+        </is>
+      </c>
+      <c r="O129" t="inlineStr">
+        <is>
+          <t>41-41</t>
+        </is>
+      </c>
+      <c r="P129" t="inlineStr">
+        <is>
+          <t>42-42</t>
+        </is>
+      </c>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>43-43</t>
+        </is>
+      </c>
+      <c r="R129" t="inlineStr">
+        <is>
+          <t>44-44</t>
+        </is>
+      </c>
+      <c r="S129" t="inlineStr">
+        <is>
+          <t>45-45</t>
+        </is>
+      </c>
+      <c r="T129" t="inlineStr">
+        <is>
+          <t>46-46</t>
+        </is>
+      </c>
+      <c r="U129" t="inlineStr">
+        <is>
+          <t>47-47</t>
         </is>
       </c>
     </row>
@@ -3553,41 +3470,65 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="E130" t="n">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="F130" t="n">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="G130" t="n">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="H130" t="n">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="I130" t="n">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="J130" t="n">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="K130" t="n">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="L130" t="n">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="M130" t="n">
-        <v>104</v>
+        <v>39</v>
+      </c>
+      <c r="N130" t="n">
+        <v>40</v>
+      </c>
+      <c r="O130" t="n">
+        <v>41</v>
+      </c>
+      <c r="P130" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q130" t="n">
+        <v>43</v>
+      </c>
+      <c r="R130" t="n">
+        <v>44</v>
+      </c>
+      <c r="S130" t="n">
+        <v>45</v>
+      </c>
+      <c r="T130" t="n">
+        <v>46</v>
+      </c>
+      <c r="U130" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr"/>
       <c r="B131" t="inlineStr">
         <is>
-          <t>CENGCENG</t>
+          <t>UGAL</t>
         </is>
       </c>
     </row>
@@ -3601,12 +3542,57 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>CENGCENG OPEN OPEN</t>
+          <t>Global</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>CENGCENG MUTED OPEN</t>
+          <t>UGAL DONG OPEN</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>UGAL DENG OPEN</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>UGAL DUNG OPEN</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>UGAL DANG OPEN</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>UGAL DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>UGAL DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>UGAL DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>UGAL DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>UGAL DANG1 OPEN</t>
+        </is>
+      </c>
+      <c r="N132" t="inlineStr">
+        <is>
+          <t>UGAL DING2 OPEN</t>
         </is>
       </c>
     </row>
@@ -3620,12 +3606,52 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>5-5</t>
+          <t>95-95</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>6-6</t>
+          <t>96-96</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>97-97</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>98-98</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>99-99</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>100-100</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>101-101</t>
+        </is>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>102-102</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>103-103</t>
+        </is>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>104-104</t>
         </is>
       </c>
     </row>
@@ -3638,10 +3664,34 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="E134" t="n">
-        <v>6</v>
+        <v>96</v>
+      </c>
+      <c r="F134" t="n">
+        <v>97</v>
+      </c>
+      <c r="G134" t="n">
+        <v>98</v>
+      </c>
+      <c r="H134" t="n">
+        <v>99</v>
+      </c>
+      <c r="I134" t="n">
+        <v>100</v>
+      </c>
+      <c r="J134" t="n">
+        <v>101</v>
+      </c>
+      <c r="K134" t="n">
+        <v>102</v>
+      </c>
+      <c r="L134" t="n">
+        <v>103</v>
+      </c>
+      <c r="M134" t="n">
+        <v>104</v>
       </c>
     </row>
     <row r="135">
@@ -3653,6 +3703,172 @@
       <c r="F135" s="2" t="n"/>
       <c r="G135" s="2" t="n"/>
     </row>
+    <row r="136">
+      <c r="A136" s="1" t="inlineStr">
+        <is>
+          <t>Presets</t>
+        </is>
+      </c>
+      <c r="B136" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C136" s="1" t="inlineStr">
+        <is>
+          <t>Generators</t>
+        </is>
+      </c>
+      <c r="D136" s="1" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="E136" s="1" t="inlineStr">
+        <is>
+          <t>Preset</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr"/>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Gong Kebyar melodic</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr"/>
+      <c r="B138" t="inlineStr"/>
+      <c r="C138" s="1" t="inlineStr">
+        <is>
+          <t>Instrument name</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>JEGOGAN</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>CALUNG</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>PENYACAH</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>PEMADE</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>KANTILAN</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>UGAL</t>
+        </is>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>GENDERRAMBAT</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>REYONG</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>TROMPONG</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr"/>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Gong Kebyar percussion</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr"/>
+      <c r="D139" t="n">
+        <v>128</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr"/>
+      <c r="B140" t="inlineStr"/>
+      <c r="C140" s="1" t="inlineStr">
+        <is>
+          <t>Instrument name</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>GONGS</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>KEMPLI</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>CENGCENG</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>KENDANG</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="inlineStr">
+        <is>
+          <t>End of data</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n"/>
+      <c r="B142" s="2" t="n"/>
+      <c r="C142" s="2" t="n"/>
+      <c r="D142" s="2" t="n"/>
+      <c r="E142" s="2" t="n"/>
+      <c r="F142" s="2" t="n"/>
+      <c r="G142" s="2" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>